<commit_message>
Starting adding tests to performance database. Added prescriptive analysis for achieving target metrics
</commit_message>
<xml_diff>
--- a/Test_Data/1-23/results/TvDNI plot.xlsx
+++ b/Test_Data/1-23/results/TvDNI plot.xlsx
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1846"/>
+  <dimension ref="A1:C1958"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -20692,6 +20692,1007 @@
         <v>14.407</v>
       </c>
     </row>
+    <row r="1847" spans="1:3">
+      <c r="A1847" s="1">
+        <v>461.2497333333332</v>
+      </c>
+      <c r="B1847">
+        <v>441.2768041237113</v>
+      </c>
+      <c r="C1847">
+        <v>14.24333333333333</v>
+      </c>
+    </row>
+    <row r="1848" spans="1:3">
+      <c r="A1848" s="1">
+        <v>461.4997333333332</v>
+      </c>
+      <c r="B1848">
+        <v>310.5088917525773</v>
+      </c>
+      <c r="C1848">
+        <v>14.55666666666667</v>
+      </c>
+    </row>
+    <row r="1849" spans="1:3">
+      <c r="A1849" s="1">
+        <v>461.7498000000001</v>
+      </c>
+      <c r="B1849">
+        <v>193.4444587628866</v>
+      </c>
+      <c r="C1849">
+        <v>14.41466666666667</v>
+      </c>
+    </row>
+    <row r="1850" spans="1:3">
+      <c r="A1850" s="1">
+        <v>461.9997333333332</v>
+      </c>
+      <c r="B1850">
+        <v>85.19974226804123</v>
+      </c>
+      <c r="C1850">
+        <v>14.42533333333333</v>
+      </c>
+    </row>
+    <row r="1851" spans="1:3">
+      <c r="A1851" s="1">
+        <v>462.2497333333334</v>
+      </c>
+      <c r="B1851">
+        <v>20.58994845360824</v>
+      </c>
+      <c r="C1851">
+        <v>14.46366666666666</v>
+      </c>
+    </row>
+    <row r="1852" spans="1:3">
+      <c r="A1852" s="1">
+        <v>462.4997333333334</v>
+      </c>
+      <c r="B1852">
+        <v>3.644072164948454</v>
+      </c>
+      <c r="C1852">
+        <v>14.35733333333334</v>
+      </c>
+    </row>
+    <row r="1853" spans="1:3">
+      <c r="A1853" s="1">
+        <v>462.7497333333333</v>
+      </c>
+      <c r="B1853">
+        <v>2.899871134020619</v>
+      </c>
+      <c r="C1853">
+        <v>14.21966666666666</v>
+      </c>
+    </row>
+    <row r="1854" spans="1:3">
+      <c r="A1854" s="1">
+        <v>462.9997333333333</v>
+      </c>
+      <c r="B1854">
+        <v>3.404510309278351</v>
+      </c>
+      <c r="C1854">
+        <v>14.08499999999999</v>
+      </c>
+    </row>
+    <row r="1855" spans="1:3">
+      <c r="A1855" s="1">
+        <v>463.2498166666665</v>
+      </c>
+      <c r="B1855">
+        <v>3.66971649484536</v>
+      </c>
+      <c r="C1855">
+        <v>14.05533333333333</v>
+      </c>
+    </row>
+    <row r="1856" spans="1:3">
+      <c r="A1856" s="1">
+        <v>463.4997333333333</v>
+      </c>
+      <c r="B1856">
+        <v>3.319072164948453</v>
+      </c>
+      <c r="C1856">
+        <v>14.219</v>
+      </c>
+    </row>
+    <row r="1857" spans="1:3">
+      <c r="A1857" s="1">
+        <v>463.7497333333333</v>
+      </c>
+      <c r="B1857">
+        <v>3.147938144329897</v>
+      </c>
+      <c r="C1857">
+        <v>14.35033333333333</v>
+      </c>
+    </row>
+    <row r="1858" spans="1:3">
+      <c r="A1858" s="1">
+        <v>463.9997999999999</v>
+      </c>
+      <c r="B1858">
+        <v>2.822938144329897</v>
+      </c>
+      <c r="C1858">
+        <v>14.255</v>
+      </c>
+    </row>
+    <row r="1859" spans="1:3">
+      <c r="A1859" s="1">
+        <v>464.2497333333333</v>
+      </c>
+      <c r="B1859">
+        <v>2.532087628865979</v>
+      </c>
+      <c r="C1859">
+        <v>14.37533333333333</v>
+      </c>
+    </row>
+    <row r="1860" spans="1:3">
+      <c r="A1860" s="1">
+        <v>464.4998166666667</v>
+      </c>
+      <c r="B1860">
+        <v>2.215592783505155</v>
+      </c>
+      <c r="C1860">
+        <v>14.13933333333334</v>
+      </c>
+    </row>
+    <row r="1861" spans="1:3">
+      <c r="A1861" s="1">
+        <v>464.7497333333332</v>
+      </c>
+      <c r="B1861">
+        <v>2.130025773195876</v>
+      </c>
+      <c r="C1861">
+        <v>14.31233333333334</v>
+      </c>
+    </row>
+    <row r="1862" spans="1:3">
+      <c r="A1862" s="1">
+        <v>465.00395</v>
+      </c>
+      <c r="B1862">
+        <v>2.232603092783505</v>
+      </c>
+      <c r="C1862">
+        <v>14.52433333333334</v>
+      </c>
+    </row>
+    <row r="1863" spans="1:3">
+      <c r="A1863" s="1">
+        <v>465.2524333333332</v>
+      </c>
+      <c r="B1863">
+        <v>2.12139175257732</v>
+      </c>
+      <c r="C1863">
+        <v>14.191</v>
+      </c>
+    </row>
+    <row r="1864" spans="1:3">
+      <c r="A1864" s="1">
+        <v>465.5009499999999</v>
+      </c>
+      <c r="B1864">
+        <v>1.804896907216495</v>
+      </c>
+      <c r="C1864">
+        <v>14.263</v>
+      </c>
+    </row>
+    <row r="1865" spans="1:3">
+      <c r="A1865" s="1">
+        <v>465.7497333333332</v>
+      </c>
+      <c r="B1865">
+        <v>1.479896907216495</v>
+      </c>
+      <c r="C1865">
+        <v>14.42966666666667</v>
+      </c>
+    </row>
+    <row r="1866" spans="1:3">
+      <c r="A1866" s="1">
+        <v>465.9997833333333</v>
+      </c>
+      <c r="B1866">
+        <v>1.197551546391752</v>
+      </c>
+      <c r="C1866">
+        <v>14.429</v>
+      </c>
+    </row>
+    <row r="1867" spans="1:3">
+      <c r="A1867" s="1">
+        <v>466.2497333333334</v>
+      </c>
+      <c r="B1867">
+        <v>1.308762886597938</v>
+      </c>
+      <c r="C1867">
+        <v>13.80866666666666</v>
+      </c>
+    </row>
+    <row r="1868" spans="1:3">
+      <c r="A1868" s="1">
+        <v>466.4998</v>
+      </c>
+      <c r="B1868">
+        <v>1.120618556701031</v>
+      </c>
+      <c r="C1868">
+        <v>14.20166666666666</v>
+      </c>
+    </row>
+    <row r="1869" spans="1:3">
+      <c r="A1869" s="1">
+        <v>466.7497333333333</v>
+      </c>
+      <c r="B1869">
+        <v>0.940979381443299</v>
+      </c>
+      <c r="C1869">
+        <v>14.06233333333334</v>
+      </c>
+    </row>
+    <row r="1870" spans="1:3">
+      <c r="A1870" s="1">
+        <v>466.9997499999999</v>
+      </c>
+      <c r="B1870">
+        <v>0.6586340206185567</v>
+      </c>
+      <c r="C1870">
+        <v>13.628</v>
+      </c>
+    </row>
+    <row r="1871" spans="1:3">
+      <c r="A1871" s="1">
+        <v>467.2498166666667</v>
+      </c>
+      <c r="B1871">
+        <v>0.581701030927835</v>
+      </c>
+      <c r="C1871">
+        <v>13.19466666666667</v>
+      </c>
+    </row>
+    <row r="1872" spans="1:3">
+      <c r="A1872" s="1">
+        <v>467.4997333333333</v>
+      </c>
+      <c r="B1872">
+        <v>0.5474226804123711</v>
+      </c>
+      <c r="C1872">
+        <v>13.017</v>
+      </c>
+    </row>
+    <row r="1873" spans="1:3">
+      <c r="A1873" s="1">
+        <v>467.7497999999999</v>
+      </c>
+      <c r="B1873">
+        <v>0.8041237113402062</v>
+      </c>
+      <c r="C1873">
+        <v>12.89333333333333</v>
+      </c>
+    </row>
+    <row r="1874" spans="1:3">
+      <c r="A1874" s="1">
+        <v>467.9997333333333</v>
+      </c>
+      <c r="B1874">
+        <v>0.8297680412371133</v>
+      </c>
+      <c r="C1874">
+        <v>13.003</v>
+      </c>
+    </row>
+    <row r="1875" spans="1:3">
+      <c r="A1875" s="1">
+        <v>468.2497333333333</v>
+      </c>
+      <c r="B1875">
+        <v>0.7185567010309278</v>
+      </c>
+      <c r="C1875">
+        <v>13.02866666666666</v>
+      </c>
+    </row>
+    <row r="1876" spans="1:3">
+      <c r="A1876" s="1">
+        <v>468.4997333333332</v>
+      </c>
+      <c r="B1876">
+        <v>0.5132731958762886</v>
+      </c>
+      <c r="C1876">
+        <v>13.14033333333333</v>
+      </c>
+    </row>
+    <row r="1877" spans="1:3">
+      <c r="A1877" s="1">
+        <v>468.7497333333332</v>
+      </c>
+      <c r="B1877">
+        <v>0.3677835051546391</v>
+      </c>
+      <c r="C1877">
+        <v>13.37733333333334</v>
+      </c>
+    </row>
+    <row r="1878" spans="1:3">
+      <c r="A1878" s="1">
+        <v>468.9997999999998</v>
+      </c>
+      <c r="B1878">
+        <v>0.2480670103092784</v>
+      </c>
+      <c r="C1878">
+        <v>13.49066666666667</v>
+      </c>
+    </row>
+    <row r="1879" spans="1:3">
+      <c r="A1879" s="1">
+        <v>469.2497666666665</v>
+      </c>
+      <c r="B1879">
+        <v>0.1453608247422681</v>
+      </c>
+      <c r="C1879">
+        <v>13.44566666666666</v>
+      </c>
+    </row>
+    <row r="1880" spans="1:3">
+      <c r="A1880" s="1">
+        <v>469.4997333333332</v>
+      </c>
+      <c r="B1880">
+        <v>0.2565721649484536</v>
+      </c>
+      <c r="C1880">
+        <v>13.609</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:3">
+      <c r="A1881" s="1">
+        <v>469.7498166666666</v>
+      </c>
+      <c r="B1881">
+        <v>0.1967783505154639</v>
+      </c>
+      <c r="C1881">
+        <v>13.64366666666667</v>
+      </c>
+    </row>
+    <row r="1882" spans="1:3">
+      <c r="A1882" s="1">
+        <v>469.9997333333334</v>
+      </c>
+      <c r="C1882">
+        <v>13.629</v>
+      </c>
+    </row>
+    <row r="1883" spans="1:3">
+      <c r="A1883" s="1">
+        <v>470.2497333333333</v>
+      </c>
+      <c r="C1883">
+        <v>13.83133333333334</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:3">
+      <c r="A1884" s="1">
+        <v>470.4997333333333</v>
+      </c>
+      <c r="C1884">
+        <v>13.77866666666667</v>
+      </c>
+    </row>
+    <row r="1885" spans="1:3">
+      <c r="A1885" s="1">
+        <v>470.7497333333333</v>
+      </c>
+      <c r="C1885">
+        <v>13.31633333333334</v>
+      </c>
+    </row>
+    <row r="1886" spans="1:3">
+      <c r="A1886" s="1">
+        <v>470.9997499999998</v>
+      </c>
+      <c r="C1886">
+        <v>12.89766666666667</v>
+      </c>
+    </row>
+    <row r="1887" spans="1:3">
+      <c r="A1887" s="1">
+        <v>471.2497333333333</v>
+      </c>
+      <c r="C1887">
+        <v>12.24466666666667</v>
+      </c>
+    </row>
+    <row r="1888" spans="1:3">
+      <c r="A1888" s="1">
+        <v>471.4997333333333</v>
+      </c>
+      <c r="C1888">
+        <v>11.46333333333333</v>
+      </c>
+    </row>
+    <row r="1889" spans="1:3">
+      <c r="A1889" s="1">
+        <v>471.7497666666666</v>
+      </c>
+      <c r="C1889">
+        <v>10.33066666666667</v>
+      </c>
+    </row>
+    <row r="1890" spans="1:3">
+      <c r="A1890" s="1">
+        <v>471.9997333333333</v>
+      </c>
+      <c r="C1890">
+        <v>9.125666666666671</v>
+      </c>
+    </row>
+    <row r="1891" spans="1:3">
+      <c r="A1891" s="1">
+        <v>472.24975</v>
+      </c>
+      <c r="C1891">
+        <v>8.065333333333328</v>
+      </c>
+    </row>
+    <row r="1892" spans="1:3">
+      <c r="A1892" s="1">
+        <v>472.4997833333333</v>
+      </c>
+      <c r="C1892">
+        <v>7.063333333333333</v>
+      </c>
+    </row>
+    <row r="1893" spans="1:3">
+      <c r="A1893" s="1">
+        <v>472.7497333333332</v>
+      </c>
+      <c r="C1893">
+        <v>5.945999999999994</v>
+      </c>
+    </row>
+    <row r="1894" spans="1:3">
+      <c r="A1894" s="1">
+        <v>472.9998000000001</v>
+      </c>
+      <c r="C1894">
+        <v>4.903666666666677</v>
+      </c>
+    </row>
+    <row r="1895" spans="1:3">
+      <c r="A1895" s="1">
+        <v>473.2497333333332</v>
+      </c>
+      <c r="C1895">
+        <v>3.625333333333334</v>
+      </c>
+    </row>
+    <row r="1896" spans="1:3">
+      <c r="A1896" s="1">
+        <v>473.4997333333334</v>
+      </c>
+      <c r="C1896">
+        <v>2.788666666666668</v>
+      </c>
+    </row>
+    <row r="1897" spans="1:3">
+      <c r="A1897" s="1">
+        <v>473.7497333333334</v>
+      </c>
+      <c r="C1897">
+        <v>2.193000000000001</v>
+      </c>
+    </row>
+    <row r="1898" spans="1:3">
+      <c r="A1898" s="1">
+        <v>473.9997333333333</v>
+      </c>
+      <c r="C1898">
+        <v>2.002333333333333</v>
+      </c>
+    </row>
+    <row r="1899" spans="1:3">
+      <c r="A1899" s="1">
+        <v>474.2497833333332</v>
+      </c>
+      <c r="C1899">
+        <v>1.773666666666667</v>
+      </c>
+    </row>
+    <row r="1900" spans="1:3">
+      <c r="A1900" s="1">
+        <v>474.4997333333333</v>
+      </c>
+      <c r="C1900">
+        <v>1.671666666666663</v>
+      </c>
+    </row>
+    <row r="1901" spans="1:3">
+      <c r="A1901" s="1">
+        <v>474.7498166666667</v>
+      </c>
+      <c r="C1901">
+        <v>1.515000000000001</v>
+      </c>
+    </row>
+    <row r="1902" spans="1:3">
+      <c r="A1902" s="1">
+        <v>474.9997333333333</v>
+      </c>
+      <c r="C1902">
+        <v>1.391999999999999</v>
+      </c>
+    </row>
+    <row r="1903" spans="1:3">
+      <c r="A1903" s="1">
+        <v>475.2497333333333</v>
+      </c>
+      <c r="C1903">
+        <v>1.257999999999999</v>
+      </c>
+    </row>
+    <row r="1904" spans="1:3">
+      <c r="A1904" s="1">
+        <v>475.4997333333333</v>
+      </c>
+      <c r="C1904">
+        <v>1.094999999999999</v>
+      </c>
+    </row>
+    <row r="1905" spans="1:3">
+      <c r="A1905" s="1">
+        <v>475.7498166666667</v>
+      </c>
+      <c r="C1905">
+        <v>0.9669999999999952</v>
+      </c>
+    </row>
+    <row r="1906" spans="1:3">
+      <c r="A1906" s="1">
+        <v>475.9997333333332</v>
+      </c>
+      <c r="C1906">
+        <v>0.7516666666666652</v>
+      </c>
+    </row>
+    <row r="1907" spans="1:3">
+      <c r="A1907" s="1">
+        <v>476.24975</v>
+      </c>
+      <c r="C1907">
+        <v>0.6396666666666633</v>
+      </c>
+    </row>
+    <row r="1908" spans="1:3">
+      <c r="A1908" s="1">
+        <v>476.4997333333332</v>
+      </c>
+      <c r="C1908">
+        <v>0.4913333333333334</v>
+      </c>
+    </row>
+    <row r="1909" spans="1:3">
+      <c r="A1909" s="1">
+        <v>476.7498000000001</v>
+      </c>
+      <c r="C1909">
+        <v>0.416999999999998</v>
+      </c>
+    </row>
+    <row r="1910" spans="1:3">
+      <c r="A1910" s="1">
+        <v>476.9997333333332</v>
+      </c>
+      <c r="C1910">
+        <v>0.3343333333333334</v>
+      </c>
+    </row>
+    <row r="1911" spans="1:3">
+      <c r="A1911" s="1">
+        <v>477.2497833333333</v>
+      </c>
+      <c r="C1911">
+        <v>0.2763333333333371</v>
+      </c>
+    </row>
+    <row r="1912" spans="1:3">
+      <c r="A1912" s="1">
+        <v>477.4997333333334</v>
+      </c>
+      <c r="C1912">
+        <v>0.2199999999999989</v>
+      </c>
+    </row>
+    <row r="1913" spans="1:3">
+      <c r="A1913" s="1">
+        <v>477.7498</v>
+      </c>
+      <c r="C1913">
+        <v>0.1373333333333342</v>
+      </c>
+    </row>
+    <row r="1914" spans="1:3">
+      <c r="A1914" s="1">
+        <v>477.9997333333333</v>
+      </c>
+      <c r="C1914">
+        <v>0.02799999999999869</v>
+      </c>
+    </row>
+    <row r="1915" spans="1:3">
+      <c r="A1915" s="1">
+        <v>478.2498166666665</v>
+      </c>
+      <c r="C1915">
+        <v>0.0313333333333361</v>
+      </c>
+    </row>
+    <row r="1916" spans="1:3">
+      <c r="A1916" s="1">
+        <v>478.4997333333333</v>
+      </c>
+      <c r="C1916">
+        <v>-0.02033333333333331</v>
+      </c>
+    </row>
+    <row r="1917" spans="1:3">
+      <c r="A1917" s="1">
+        <v>478.7497833333334</v>
+      </c>
+      <c r="C1917">
+        <v>-0.1350000000000016</v>
+      </c>
+    </row>
+    <row r="1918" spans="1:3">
+      <c r="A1918" s="1">
+        <v>478.9997333333333</v>
+      </c>
+      <c r="C1918">
+        <v>-0.2119999999999997</v>
+      </c>
+    </row>
+    <row r="1919" spans="1:3">
+      <c r="A1919" s="1">
+        <v>479.2497333333333</v>
+      </c>
+      <c r="C1919">
+        <v>-0.1906666666666652</v>
+      </c>
+    </row>
+    <row r="1920" spans="1:3">
+      <c r="A1920" s="1">
+        <v>479.4997333333333</v>
+      </c>
+      <c r="C1920">
+        <v>-0.1506666666666661</v>
+      </c>
+    </row>
+    <row r="1921" spans="1:3">
+      <c r="A1921" s="1">
+        <v>479.7497833333333</v>
+      </c>
+      <c r="C1921">
+        <v>-0.1333333333333293</v>
+      </c>
+    </row>
+    <row r="1922" spans="1:3">
+      <c r="A1922" s="1">
+        <v>479.9997333333332</v>
+      </c>
+      <c r="C1922">
+        <v>-0.2056666666666658</v>
+      </c>
+    </row>
+    <row r="1923" spans="1:3">
+      <c r="A1923" s="1">
+        <v>480.2497333333332</v>
+      </c>
+      <c r="C1923">
+        <v>-0.251333333333335</v>
+      </c>
+    </row>
+    <row r="1924" spans="1:3">
+      <c r="A1924" s="1">
+        <v>480.4998000000001</v>
+      </c>
+      <c r="C1924">
+        <v>-0.2966666666666633</v>
+      </c>
+    </row>
+    <row r="1925" spans="1:3">
+      <c r="A1925" s="1">
+        <v>480.7497333333332</v>
+      </c>
+      <c r="C1925">
+        <v>-0.1990000000000016</v>
+      </c>
+    </row>
+    <row r="1926" spans="1:3">
+      <c r="A1926" s="1">
+        <v>480.9997833333333</v>
+      </c>
+      <c r="C1926">
+        <v>-0.3256666666666668</v>
+      </c>
+    </row>
+    <row r="1927" spans="1:3">
+      <c r="A1927" s="1">
+        <v>481.2497333333334</v>
+      </c>
+      <c r="C1927">
+        <v>-0.3006666666666682</v>
+      </c>
+    </row>
+    <row r="1928" spans="1:3">
+      <c r="A1928" s="1">
+        <v>481.4997666666667</v>
+      </c>
+      <c r="C1928">
+        <v>-0.396333333333331</v>
+      </c>
+    </row>
+    <row r="1929" spans="1:3">
+      <c r="A1929" s="1">
+        <v>481.7497333333333</v>
+      </c>
+      <c r="C1929">
+        <v>-0.4209999999999994</v>
+      </c>
+    </row>
+    <row r="1930" spans="1:3">
+      <c r="A1930" s="1">
+        <v>481.9997333333333</v>
+      </c>
+      <c r="C1930">
+        <v>-0.320333333333334</v>
+      </c>
+    </row>
+    <row r="1931" spans="1:3">
+      <c r="A1931" s="1">
+        <v>482.2498166666667</v>
+      </c>
+      <c r="C1931">
+        <v>-0.3866666666666667</v>
+      </c>
+    </row>
+    <row r="1932" spans="1:3">
+      <c r="A1932" s="1">
+        <v>482.4997333333333</v>
+      </c>
+      <c r="C1932">
+        <v>-0.3989999999999974</v>
+      </c>
+    </row>
+    <row r="1933" spans="1:3">
+      <c r="A1933" s="1">
+        <v>482.7497333333333</v>
+      </c>
+      <c r="C1933">
+        <v>-0.3926666666666669</v>
+      </c>
+    </row>
+    <row r="1934" spans="1:3">
+      <c r="A1934" s="1">
+        <v>482.9997333333333</v>
+      </c>
+      <c r="C1934">
+        <v>-0.3466666666666676</v>
+      </c>
+    </row>
+    <row r="1935" spans="1:3">
+      <c r="A1935" s="1">
+        <v>483.2497833333333</v>
+      </c>
+      <c r="C1935">
+        <v>-0.378666666666664</v>
+      </c>
+    </row>
+    <row r="1936" spans="1:3">
+      <c r="A1936" s="1">
+        <v>483.4998166666667</v>
+      </c>
+      <c r="C1936">
+        <v>-0.4083333333333314</v>
+      </c>
+    </row>
+    <row r="1937" spans="1:3">
+      <c r="A1937" s="1">
+        <v>483.7497333333332</v>
+      </c>
+      <c r="C1937">
+        <v>-0.4260000000000055</v>
+      </c>
+    </row>
+    <row r="1938" spans="1:3">
+      <c r="A1938" s="1">
+        <v>483.9997666666665</v>
+      </c>
+      <c r="C1938">
+        <v>-0.3840000000000003</v>
+      </c>
+    </row>
+    <row r="1939" spans="1:3">
+      <c r="A1939" s="1">
+        <v>484.2497333333332</v>
+      </c>
+      <c r="C1939">
+        <v>-0.3853333333333353</v>
+      </c>
+    </row>
+    <row r="1940" spans="1:3">
+      <c r="A1940" s="1">
+        <v>484.4997499999999</v>
+      </c>
+      <c r="C1940">
+        <v>-0.4140000000000015</v>
+      </c>
+    </row>
+    <row r="1941" spans="1:3">
+      <c r="A1941" s="1">
+        <v>484.7497833333333</v>
+      </c>
+      <c r="C1941">
+        <v>-0.3880000000000017</v>
+      </c>
+    </row>
+    <row r="1942" spans="1:3">
+      <c r="A1942" s="1">
+        <v>484.9997333333334</v>
+      </c>
+      <c r="C1942">
+        <v>-0.3860000000000028</v>
+      </c>
+    </row>
+    <row r="1943" spans="1:3">
+      <c r="A1943" s="1">
+        <v>485.2497666666667</v>
+      </c>
+      <c r="C1943">
+        <v>-0.4506666666666668</v>
+      </c>
+    </row>
+    <row r="1944" spans="1:3">
+      <c r="A1944" s="1">
+        <v>485.4997333333333</v>
+      </c>
+      <c r="C1944">
+        <v>-0.4106666666666676</v>
+      </c>
+    </row>
+    <row r="1945" spans="1:3">
+      <c r="A1945" s="1">
+        <v>485.7497499999999</v>
+      </c>
+      <c r="C1945">
+        <v>-0.3816666666666677</v>
+      </c>
+    </row>
+    <row r="1946" spans="1:3">
+      <c r="A1946" s="1">
+        <v>485.9997333333333</v>
+      </c>
+      <c r="C1946">
+        <v>-0.3866666666666667</v>
+      </c>
+    </row>
+    <row r="1947" spans="1:3">
+      <c r="A1947" s="1">
+        <v>486.2497499999998</v>
+      </c>
+      <c r="C1947">
+        <v>-0.3153333333333386</v>
+      </c>
+    </row>
+    <row r="1948" spans="1:3">
+      <c r="A1948" s="1">
+        <v>486.4997333333333</v>
+      </c>
+      <c r="C1948">
+        <v>-0.277666666666665</v>
+      </c>
+    </row>
+    <row r="1949" spans="1:3">
+      <c r="A1949" s="1">
+        <v>486.7497999999999</v>
+      </c>
+      <c r="C1949">
+        <v>-0.3026666666666671</v>
+      </c>
+    </row>
+    <row r="1950" spans="1:3">
+      <c r="A1950" s="1">
+        <v>486.9997333333333</v>
+      </c>
+      <c r="C1950">
+        <v>-0.277000000000001</v>
+      </c>
+    </row>
+    <row r="1951" spans="1:3">
+      <c r="A1951" s="1">
+        <v>487.2498166666667</v>
+      </c>
+      <c r="C1951">
+        <v>-0.277000000000001</v>
+      </c>
+    </row>
+    <row r="1952" spans="1:3">
+      <c r="A1952" s="1">
+        <v>487.4997333333332</v>
+      </c>
+      <c r="C1952">
+        <v>-0.1986666666666643</v>
+      </c>
+    </row>
+    <row r="1953" spans="1:3">
+      <c r="A1953" s="1">
+        <v>487.7497999999998</v>
+      </c>
+      <c r="C1953">
+        <v>-0.2473333333333301</v>
+      </c>
+    </row>
+    <row r="1954" spans="1:3">
+      <c r="A1954" s="1">
+        <v>487.9998000000001</v>
+      </c>
+      <c r="C1954">
+        <v>-0.1993333333333354</v>
+      </c>
+    </row>
+    <row r="1955" spans="1:3">
+      <c r="A1955" s="1">
+        <v>488.2498166666666</v>
+      </c>
+      <c r="C1955">
+        <v>-0.2013333333333343</v>
+      </c>
+    </row>
+    <row r="1956" spans="1:3">
+      <c r="A1956" s="1">
+        <v>488.4997333333334</v>
+      </c>
+      <c r="C1956">
+        <v>-0.2360000000000007</v>
+      </c>
+    </row>
+    <row r="1957" spans="1:3">
+      <c r="A1957" s="1">
+        <v>488.7497333333334</v>
+      </c>
+      <c r="C1957">
+        <v>-0.2070000000000007</v>
+      </c>
+    </row>
+    <row r="1958" spans="1:3">
+      <c r="A1958" s="1">
+        <v>488.9997333333333</v>
+      </c>
+      <c r="C1958">
+        <v>-0.1166666666666671</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>